<commit_message>
updated readme and data
</commit_message>
<xml_diff>
--- a/birthday-prabhuji.xlsx
+++ b/birthday-prabhuji.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\iskcon\birthday notifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CD111F-B7D3-4821-A84C-A3435B26F0FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A51436-AE18-4656-AD58-F32A116A5800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{ABD2D5D9-8F7D-47F9-A563-F3C75A0C7FA9}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -538,6 +538,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F3F58B-7785-4D60-BB2A-857ECE00E0A2}">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1771,7 +1774,10 @@
       </c>
       <c r="C62" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>00-01-1900</v>
+        <v>06-04-2004</v>
+      </c>
+      <c r="D62" s="25">
+        <v>38083</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added sample excel file
</commit_message>
<xml_diff>
--- a/birthday-prabhuji.xlsx
+++ b/birthday-prabhuji.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\iskcon\birthday notifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A51436-AE18-4656-AD58-F32A116A5800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0AE8B2-40B8-4708-9E12-E5523D8D94B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{ABD2D5D9-8F7D-47F9-A563-F3C75A0C7FA9}"/>
   </bookViews>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F3F58B-7785-4D60-BB2A-857ECE00E0A2}">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1791,6 +1791,7 @@
         <f t="shared" si="1"/>
         <v>00-01-1900</v>
       </c>
+      <c r="D63" s="25"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="16" t="s">
@@ -1803,8 +1804,9 @@
         <f t="shared" si="1"/>
         <v>00-01-1900</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64" s="25"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="14" t="s">
         <v>71</v>
       </c>
@@ -1815,8 +1817,9 @@
         <f t="shared" si="1"/>
         <v>00-01-1900</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65" s="25"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="14" t="s">
         <v>93</v>
       </c>
@@ -1827,8 +1830,9 @@
         <f t="shared" ref="C66:C67" si="2">TEXT(D66,"dd-mm-yyyy")</f>
         <v>00-01-1900</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66" s="25"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="14" t="s">
         <v>94</v>
       </c>
@@ -1839,6 +1843,7 @@
         <f t="shared" si="2"/>
         <v>00-01-1900</v>
       </c>
+      <c r="D67" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D60">

</xml_diff>